<commit_message>
Update infor for new version 1.4.1
</commit_message>
<xml_diff>
--- a/.github/assets/tableConvert.com_e6av2l.xlsx
+++ b/.github/assets/tableConvert.com_e6av2l.xlsx
@@ -5,16 +5,16 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\libs\permetrics\.github\img\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\libs\permetrics\.github\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13572" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="classification" sheetId="2" r:id="rId2"/>
+    <sheet name="clustering" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="277">
   <si>
     <t>**Problem**</t>
   </si>
@@ -811,6 +811,48 @@
   </si>
   <si>
     <t>Characteristics</t>
+  </si>
+  <si>
+    <t>Smaller is better (No best value), Range=(-inf, inf)</t>
+  </si>
+  <si>
+    <t>Bigger is better (No best value), Range=[0, inf)</t>
+  </si>
+  <si>
+    <t>Bigger is better (No best value), Range=[0, +inf)</t>
+  </si>
+  <si>
+    <t>Smaller is better (No best value), Range=(-inf, +inf)</t>
+  </si>
+  <si>
+    <t>Bigger is better (No best value), Range=(-inf, +inf)</t>
+  </si>
+  <si>
+    <t>Higher is better (No best value), Range = [0, +inf)</t>
+  </si>
+  <si>
+    <t>Higher is better (Best = 1), Range=[-1, +1]</t>
+  </si>
+  <si>
+    <t>Higher is better (No best value), Range=(-inf, +inf)</t>
+  </si>
+  <si>
+    <t>Higher is better (No best value), Range = (-inf, +inf)</t>
+  </si>
+  <si>
+    <t>LS</t>
+  </si>
+  <si>
+    <t>Lift Score</t>
+  </si>
+  <si>
+    <t>Smaller is better (Best = 0), Range = [0, +1]</t>
+  </si>
+  <si>
+    <t>Bigger is better (Best = 1), Range = [-1, +1]</t>
+  </si>
+  <si>
+    <t>Hamming Score</t>
   </si>
 </sst>
 </file>
@@ -1190,13 +1232,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D10" sqref="A1:E97"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection sqref="A1:E98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.19921875" customWidth="1"/>
     <col min="2" max="2" width="6.5" customWidth="1"/>
@@ -1205,7 +1247,7 @@
     <col min="5" max="5" width="50.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1222,7 +1264,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1239,7 +1281,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1256,7 +1298,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1273,7 +1315,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1290,7 +1332,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1307,7 +1349,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1324,7 +1366,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1341,7 +1383,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1358,7 +1400,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1375,7 +1417,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1392,7 +1434,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1409,7 +1451,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -1426,7 +1468,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1443,7 +1485,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -1460,7 +1502,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -1477,7 +1519,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -1494,7 +1536,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
@@ -1511,7 +1553,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -1528,7 +1570,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -1545,7 +1587,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -1562,7 +1604,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -1579,7 +1621,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
@@ -1596,7 +1638,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>10</v>
       </c>
@@ -1613,7 +1655,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
@@ -1630,7 +1672,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>10</v>
       </c>
@@ -1647,7 +1689,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
@@ -1664,7 +1706,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
@@ -1681,7 +1723,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>10</v>
       </c>
@@ -1698,7 +1740,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
@@ -1715,7 +1757,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>10</v>
       </c>
@@ -1732,7 +1774,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>10</v>
       </c>
@@ -1749,7 +1791,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
@@ -1766,7 +1808,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>10</v>
       </c>
@@ -1783,7 +1825,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
@@ -1800,7 +1842,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>10</v>
       </c>
@@ -1817,7 +1859,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>10</v>
       </c>
@@ -1834,7 +1876,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>10</v>
       </c>
@@ -1851,7 +1893,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>10</v>
       </c>
@@ -1868,7 +1910,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>10</v>
       </c>
@@ -1885,7 +1927,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>10</v>
       </c>
@@ -1902,7 +1944,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>10</v>
       </c>
@@ -1919,7 +1961,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>10</v>
       </c>
@@ -1936,7 +1978,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>10</v>
       </c>
@@ -1953,7 +1995,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>10</v>
       </c>
@@ -1970,7 +2012,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>10</v>
       </c>
@@ -1987,7 +2029,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>10</v>
       </c>
@@ -2004,7 +2046,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>10</v>
       </c>
@@ -2021,7 +2063,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>10</v>
       </c>
@@ -2038,7 +2080,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>163</v>
       </c>
@@ -2055,7 +2097,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>10</v>
       </c>
@@ -2072,7 +2114,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>10</v>
       </c>
@@ -2089,7 +2131,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>10</v>
       </c>
@@ -2106,7 +2148,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>10</v>
       </c>
@@ -2123,7 +2165,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>10</v>
       </c>
@@ -2140,7 +2182,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>10</v>
       </c>
@@ -2157,7 +2199,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>10</v>
       </c>
@@ -2174,7 +2216,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>10</v>
       </c>
@@ -2191,7 +2233,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>10</v>
       </c>
@@ -2199,16 +2241,16 @@
         <v>37</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>184</v>
+        <v>227</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>185</v>
+        <v>276</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>10</v>
       </c>
@@ -2225,7 +2267,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>10</v>
       </c>
@@ -2242,7 +2284,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>10</v>
       </c>
@@ -2259,7 +2301,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>10</v>
       </c>
@@ -2267,16 +2309,16 @@
         <v>50</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>91</v>
+        <v>195</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>10</v>
       </c>
@@ -2284,72 +2326,72 @@
         <v>53</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>195</v>
+        <v>272</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>195</v>
+        <v>273</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>10</v>
+        <v>194</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B67" s="1">
         <v>1</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E67" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B67" s="1">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68" s="1">
         <v>2</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B68" s="1">
-        <v>3</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>201</v>
@@ -2361,513 +2403,530 @@
         <v>14</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B69" s="1">
+        <v>3</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B70" s="1">
         <v>4</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D70" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E69" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B70" s="1">
+      <c r="E70" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B71" s="1">
         <v>5</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E70" s="1" t="s">
+      <c r="C71" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B72" s="1">
+        <v>6</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B73" s="1">
+        <v>7</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B74" s="1">
+        <v>8</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B75" s="1">
+        <v>9</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B76" s="1">
+        <v>10</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B77" s="1">
+        <v>11</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B78" s="1">
+        <v>12</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B79" s="1">
+        <v>13</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B80" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B71" s="1">
-        <v>6</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B72" s="1">
-        <v>7</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B73" s="1">
-        <v>8</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B74" s="1">
-        <v>9</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B75" s="1">
-        <v>10</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B76" s="1">
-        <v>11</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B77" s="1">
-        <v>12</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B78" s="1">
-        <v>13</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B79" s="1">
-        <v>14</v>
-      </c>
-      <c r="C79" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D80" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="E79" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B80" s="1">
+      <c r="E80" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B81" s="1">
         <v>15</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D81" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="E80" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B81" s="1">
+      <c r="E81" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B82" s="1">
         <v>16</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C82" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D82" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="E81" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B82" s="1">
+      <c r="E82" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B83" s="1">
         <v>17</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C83" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="D83" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="E82" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B83" s="1">
+      <c r="E83" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B84" s="1">
         <v>18</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="D84" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="E83" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A84" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B84" s="1">
+      <c r="E84" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B85" s="1">
         <v>19</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C85" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="D85" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E84" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B85" s="1">
+      <c r="E85" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B86" s="1">
         <v>20</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C86" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="D86" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E85" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B86" s="1">
+      <c r="E86" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B87" s="1">
         <v>21</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C87" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="D86" s="1" t="s">
+      <c r="D87" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="E86" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B87" s="1">
+      <c r="E87" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B88" s="1">
         <v>22</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C88" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="D88" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E87" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A88" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B88" s="1">
+      <c r="E88" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B89" s="1">
         <v>23</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C89" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="D89" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="E88" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B89" s="1">
+      <c r="E89" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B90" s="1">
         <v>24</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C90" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="D90" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="E89" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B90" s="1">
+      <c r="E90" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B91" s="1">
         <v>25</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C91" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="D91" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="E90" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A91" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B91" s="1">
+      <c r="E91" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B92" s="1">
         <v>26</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C92" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="D92" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E91" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A92" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B92" s="1">
+      <c r="E92" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B93" s="1">
         <v>27</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C93" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="D92" s="1" t="s">
+      <c r="D93" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="E92" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B93" s="1">
+      <c r="E93" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B94" s="1">
         <v>28</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C94" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="D93" s="1" t="s">
+      <c r="D94" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E93" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A94" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B94" s="1">
+      <c r="E94" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B95" s="1">
         <v>29</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C95" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="D94" s="1" t="s">
+      <c r="D95" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="E94" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A95" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B95" s="1">
+      <c r="E95" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B96" s="1">
         <v>30</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C96" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D95" s="1" t="s">
+      <c r="D96" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="E95" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A96" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B96" s="1">
+      <c r="E96" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B97" s="1">
         <v>31</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C97" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="D97" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="E96" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A97" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="E97" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E98" s="1" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E48 A50:E64 A49 A65" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:E48 A50:A64 A49 A65" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2878,7 +2937,7 @@
     <col min="4" max="4" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>259</v>
       </c>
@@ -2891,8 +2950,10 @@
       <c r="D1" s="1" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -2905,8 +2966,10 @@
       <c r="D2" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -2919,8 +2982,10 @@
       <c r="D3" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -2933,8 +2998,10 @@
       <c r="D4" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -2947,8 +3014,10 @@
       <c r="D5" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -2961,8 +3030,10 @@
       <c r="D6" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -2975,8 +3046,10 @@
       <c r="D7" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -2989,8 +3062,10 @@
       <c r="D8" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -3003,8 +3078,10 @@
       <c r="D9" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
@@ -3017,22 +3094,26 @@
       <c r="D10" s="1" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>184</v>
+        <v>227</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>185</v>
+        <v>276</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
@@ -3045,8 +3126,10 @@
       <c r="D12" s="1" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -3059,8 +3142,10 @@
       <c r="D13" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>47</v>
       </c>
@@ -3073,37 +3158,62 @@
       <c r="D14" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>91</v>
+        <v>195</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>195</v>
+        <v>272</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>195</v>
+        <v>273</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>191</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3111,8 +3221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3155,13 +3265,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>257</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3169,10 +3279,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>14</v>
@@ -3189,7 +3299,7 @@
         <v>204</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -3197,13 +3307,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -3217,7 +3327,7 @@
         <v>208</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>46</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -3231,7 +3341,7 @@
         <v>210</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -3239,13 +3349,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>46</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -3259,7 +3369,7 @@
         <v>214</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -3273,7 +3383,7 @@
         <v>216</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -3287,7 +3397,7 @@
         <v>218</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>183</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -3301,7 +3411,7 @@
         <v>220</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>166</v>
+        <v>268</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -3455,7 +3565,7 @@
         <v>240</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>151</v>
+        <v>269</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -3497,7 +3607,7 @@
         <v>246</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>46</v>
+        <v>270</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -3511,7 +3621,7 @@
         <v>248</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>183</v>
+        <v>271</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -3572,6 +3682,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3579,11 +3690,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D97"/>
+    <sheetView topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="20.796875" customWidth="1"/>
+    <col min="3" max="3" width="36.296875" customWidth="1"/>
+    <col min="4" max="4" width="50.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">

</xml_diff>